<commit_message>
KIBON-1138: Neue Statistik Verrechnung Tagesschulen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleRechnungsstellung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleRechnungsstellung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Transfer\kiBon-Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C28EC8-7F0E-43C2-AF8D-EF104CEE131A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367E7EEC-DF41-4EFE-AF8C-99FA4907E581}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Data" sheetId="6" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$5:$L$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$5:$L$12</definedName>
     <definedName name="angemeldet1">Data!#REF!</definedName>
     <definedName name="angemeldet10">Data!#REF!</definedName>
     <definedName name="angemeldet100">Data!#REF!</definedName>
@@ -234,49 +234,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
-  <si>
-    <t>Wälti</t>
-  </si>
-  <si>
-    <t>Simon</t>
-  </si>
-  <si>
-    <t>20.000109.001.1.3</t>
-  </si>
-  <si>
-    <t>20.000106.001.1.3</t>
-  </si>
-  <si>
-    <t>Dagmar</t>
-  </si>
-  <si>
-    <t>Testweg</t>
-  </si>
-  <si>
-    <t>Bern</t>
-  </si>
-  <si>
-    <t>Feutz</t>
-  </si>
-  <si>
-    <t>Tamara</t>
-  </si>
-  <si>
-    <t>Yvonne</t>
-  </si>
-  <si>
-    <t>Postgasse</t>
-  </si>
-  <si>
-    <t>Thun</t>
-  </si>
-  <si>
-    <t>Tagesschule Bremgarten</t>
-  </si>
-  <si>
-    <t>Tagesschule Lorraine</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>{repeatRow}</t>
   </si>
@@ -561,7 +519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -598,6 +556,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -613,16 +581,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1033,7 +994,7 @@
   <sheetPr codeName="Tabelle1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -1062,15 +1023,15 @@
   <sheetData>
     <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
-        <v>15</v>
+      <c r="A4" s="21" t="s">
+        <v>1</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C4"/>
     </row>
@@ -1094,346 +1055,187 @@
       <c r="Q5"/>
     </row>
     <row r="6" spans="1:19" s="16" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="R6" s="27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" s="16" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23"/>
+      <c r="B7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="23"/>
+      <c r="F7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="I7" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="25" t="s">
+      <c r="K7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="23"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="L8" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="M6" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="N6" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="O6" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="P6" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q6" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="R6" s="23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" s="16" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="13" t="s">
+      <c r="M8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" s="13" t="s">
+      <c r="N8" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" s="13" t="s">
+      <c r="O8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="L7" s="26"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="P8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="R8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="S8" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="6">
-        <v>41742</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" s="3">
-        <v>10</v>
-      </c>
-      <c r="J8" s="3">
-        <v>3000</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8" s="15">
-        <v>44044</v>
-      </c>
-      <c r="M8" s="7">
-        <v>53872</v>
-      </c>
-      <c r="N8" s="19">
-        <v>2</v>
-      </c>
-      <c r="O8" s="7">
-        <v>53872</v>
-      </c>
-      <c r="P8" s="4">
-        <v>44044</v>
-      </c>
-      <c r="Q8" s="14">
-        <v>1.84</v>
-      </c>
-      <c r="R8" s="14">
-        <v>1.62</v>
-      </c>
     </row>
     <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="6">
-        <v>40005</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="3">
-        <v>1</v>
-      </c>
-      <c r="J9" s="3">
-        <v>3600</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="15">
-        <v>44044</v>
-      </c>
-      <c r="M9" s="7">
-        <v>137346</v>
-      </c>
-      <c r="N9" s="19">
-        <v>2</v>
-      </c>
-      <c r="O9" s="7">
-        <v>137346</v>
-      </c>
-      <c r="P9" s="4">
-        <v>44075</v>
-      </c>
-      <c r="Q9" s="14">
-        <v>7.67</v>
-      </c>
-      <c r="R9" s="14">
-        <v>7.24</v>
-      </c>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="6">
-        <v>41742</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I10" s="3">
-        <v>10</v>
-      </c>
-      <c r="J10" s="3">
-        <v>3000</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L10" s="15">
-        <v>44075</v>
-      </c>
-      <c r="M10" s="7">
-        <v>53872</v>
-      </c>
-      <c r="N10" s="19">
-        <v>2</v>
-      </c>
-      <c r="O10" s="7">
-        <v>53872</v>
-      </c>
-      <c r="P10" s="4">
-        <v>44044</v>
-      </c>
-      <c r="Q10" s="14">
-        <v>1.84</v>
-      </c>
-      <c r="R10" s="14">
-        <v>1.62</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="C10"/>
     </row>
     <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="L11" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="N11" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q11" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="R11" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="S11" s="27" t="s">
-        <v>14</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="C11"/>
     </row>
     <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-    </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="C12"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="C13"/>
     </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="C14"/>
-    </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="C15"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="C16"/>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28"/>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C30"/>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C31"/>
@@ -1464,15 +1266,6 @@
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40"/>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C41"/>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C42"/>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C43"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1494,6 +1287,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1502,7 +1301,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100178195A6A82AF84FAFDB8827B239111E" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="f80ea4e6a0993f4123c203954d678651">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1628a9ab-243a-442a-b1b3-2e5b8f50e59d" xmlns:ns4="b65bf3a7-05af-4187-ae34-5d8f1e986b06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ee4477c2c38746f2954221b423fbb2cf" ns3:_="" ns4:_="">
     <xsd:import namespace="1628a9ab-243a-442a-b1b3-2e5b8f50e59d"/>
@@ -1705,13 +1504,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AABB69B-6189-49E4-B0B4-0F8B91A6C08D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72EE7358-3502-47F9-A7E9-E9E6E3E32984}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1719,7 +1521,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{429A54D3-D389-40FF-9DA8-392EAF9E6C57}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1736,13 +1538,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AABB69B-6189-49E4-B0B4-0F8B91A6C08D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
KIBON-1138: Korrekturen aus Review
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleRechnungsstellung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleRechnungsstellung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Transfer\kiBon-Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3A2DF1-DD81-4C60-956A-1E6034057D53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8AFEC68-CE03-4ECE-9C94-F48C466489B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{872481F4-EE12-4A1C-A697-190F599814C2}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{872481F4-EE12-4A1C-A697-190F599814C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -169,7 +169,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="&quot;CHF&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,8 +192,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +211,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -319,6 +332,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -335,9 +351,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -661,6 +674,7 @@
     <col min="1" max="1" width="16.125" customWidth="1"/>
     <col min="2" max="2" width="16.25" customWidth="1"/>
     <col min="3" max="3" width="15.25" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="15.875" customWidth="1"/>
     <col min="7" max="7" width="16.5" customWidth="1"/>
     <col min="8" max="8" width="16.25" customWidth="1"/>
@@ -681,10 +695,10 @@
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2"/>
@@ -693,49 +707,49 @@
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="11" t="s">
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="11" t="s">
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="M6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="O6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="P6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="Q6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="R6" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
@@ -745,7 +759,7 @@
       <c r="D7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="12"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="3" t="s">
         <v>17</v>
       </c>
@@ -764,13 +778,13 @@
       <c r="K7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">

</xml_diff>

<commit_message>
KIBON-1537 Erklärung Einkommen und Korrektur Datum in Template
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleRechnungsstellung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleRechnungsstellung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Transfer\kiBon-Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8AFEC68-CE03-4ECE-9C94-F48C466489B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50217819-D2BE-4175-BEF2-8621358B0002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{872481F4-EE12-4A1C-A697-190F599814C2}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12735" xr2:uid="{872481F4-EE12-4A1C-A697-190F599814C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>{tagesschuleRechungsstellungTitle}</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>{repeatRow}</t>
+  </si>
+  <si>
+    <t>{erklaerungEinkommen}</t>
+  </si>
+  <si>
+    <t>{erklaerungEinkommenTitle}</t>
   </si>
 </sst>
 </file>
@@ -310,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -332,9 +338,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -350,7 +354,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -665,7 +677,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0BAE374-0165-43F7-9727-7ADA8430C8E9}">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -679,34 +691,34 @@
     <col min="7" max="7" width="16.5" customWidth="1"/>
     <col min="8" max="8" width="16.25" customWidth="1"/>
     <col min="13" max="13" width="18.5" customWidth="1"/>
-    <col min="15" max="15" width="17.875" customWidth="1"/>
+    <col min="15" max="16" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="17" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
@@ -738,17 +750,20 @@
       <c r="O6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="P6" s="12" t="s">
+      <c r="P6" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q6" s="12" t="s">
+      <c r="R6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="R6" s="12" t="s">
+      <c r="S6" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="3" t="s">
         <v>14</v>
@@ -782,11 +797,12 @@
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
       <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
+      <c r="P7" s="19"/>
       <c r="Q7" s="13"/>
       <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -832,24 +848,27 @@
       <c r="O8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="P8" s="6" t="s">
+      <c r="P8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="Q8" s="10" t="s">
+      <c r="R8" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="R8" s="10" t="s">
+      <c r="S8" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="P6:P7"/>
+  <mergeCells count="12">
     <mergeCell ref="Q6:Q7"/>
     <mergeCell ref="R6:R7"/>
+    <mergeCell ref="S6:S7"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="L6:L7"/>
@@ -858,6 +877,7 @@
     <mergeCell ref="O6:O7"/>
     <mergeCell ref="F6:K6"/>
     <mergeCell ref="B6:D6"/>
+    <mergeCell ref="P6:P7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
KIBON-1537 PMD und Template
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleRechnungsstellung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleRechnungsstellung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50217819-D2BE-4175-BEF2-8621358B0002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FE9E84-101B-4D54-BDCB-6DF15FFCF154}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12735" xr2:uid="{872481F4-EE12-4A1C-A697-190F599814C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{872481F4-EE12-4A1C-A697-190F599814C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -316,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -339,6 +339,9 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -352,15 +355,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -710,7 +704,7 @@
       <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2"/>
@@ -719,52 +713,52 @@
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="12" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="12" t="s">
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="M6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="O6" s="12" t="s">
+      <c r="O6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="P6" s="18" t="s">
+      <c r="P6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="Q6" s="12" t="s">
+      <c r="Q6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="R6" s="12" t="s">
+      <c r="R6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="S6" s="12" t="s">
+      <c r="S6" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
@@ -774,7 +768,7 @@
       <c r="D7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="13"/>
+      <c r="E7" s="14"/>
       <c r="F7" s="3" t="s">
         <v>17</v>
       </c>
@@ -793,14 +787,14 @@
       <c r="K7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">

</xml_diff>

<commit_message>
KIBON-1863: Einkommensverschelechterung im Tagesschule Rechnungstellung addiert
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleRechnungsstellung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleRechnungsstellung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FE9E84-101B-4D54-BDCB-6DF15FFCF154}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C8212B-7512-4197-A122-2E746FB347CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{872481F4-EE12-4A1C-A697-190F599814C2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{872481F4-EE12-4A1C-A697-190F599814C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>{tagesschuleRechungsstellungTitle}</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>{erklaerungEinkommenTitle}</t>
+  </si>
+  <si>
+    <t>{einkommensverschlechterungTitle}</t>
+  </si>
+  <si>
+    <t>{einkommensverschlechterung}</t>
   </si>
 </sst>
 </file>
@@ -316,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -357,6 +363,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -671,36 +678,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0BAE374-0165-43F7-9727-7ADA8430C8E9}">
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.125" customWidth="1"/>
-    <col min="2" max="2" width="16.25" customWidth="1"/>
-    <col min="3" max="3" width="15.25" customWidth="1"/>
+    <col min="1" max="1" width="16.09765625" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" customWidth="1"/>
+    <col min="3" max="3" width="15.19921875" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="15.875" customWidth="1"/>
+    <col min="6" max="6" width="15.8984375" customWidth="1"/>
     <col min="7" max="7" width="16.5" customWidth="1"/>
-    <col min="8" max="8" width="16.25" customWidth="1"/>
+    <col min="8" max="8" width="16.19921875" customWidth="1"/>
     <col min="13" max="13" width="18.5" customWidth="1"/>
-    <col min="15" max="16" width="17.875" customWidth="1"/>
+    <col min="15" max="17" width="17.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
@@ -709,10 +718,10 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
@@ -745,19 +754,22 @@
         <v>10</v>
       </c>
       <c r="P6" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="Q6" s="13" t="s">
+      <c r="R6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="R6" s="13" t="s">
+      <c r="S6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="S6" s="13" t="s">
+      <c r="T6" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="3" t="s">
         <v>14</v>
@@ -795,8 +807,9 @@
       <c r="Q7" s="14"/>
       <c r="R7" s="14"/>
       <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -842,27 +855,30 @@
       <c r="O8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="P8" s="9" t="s">
+      <c r="P8" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="6" t="s">
+      <c r="R8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="R8" s="10" t="s">
+      <c r="S8" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="S8" s="10" t="s">
+      <c r="T8" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="Q6:Q7"/>
+  <mergeCells count="13">
     <mergeCell ref="R6:R7"/>
     <mergeCell ref="S6:S7"/>
+    <mergeCell ref="T6:T7"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="L6:L7"/>
@@ -871,8 +887,10 @@
     <mergeCell ref="O6:O7"/>
     <mergeCell ref="F6:K6"/>
     <mergeCell ref="B6:D6"/>
+    <mergeCell ref="Q6:Q7"/>
     <mergeCell ref="P6:P7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
KIBON-1968: Feld Organisation addiert bei abweichende Rechnungsadresse im GUI, im Scolaris und im TagessschuleRechnungsStati
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleRechnungsstellung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleRechnungsstellung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D0B3D7-E9BD-4260-9100-718780989053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4064F3-ACE3-47F1-BFD1-407022203760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{872481F4-EE12-4A1C-A697-190F599814C2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{872481F4-EE12-4A1C-A697-190F599814C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>{tagesschuleRechungsstellungTitle}</t>
   </si>
@@ -177,6 +177,12 @@
   </si>
   <si>
     <t>{einkommensverschlechterungAnnuliert}</t>
+  </si>
+  <si>
+    <t>{rechnungsadresseOrganisationTitle}</t>
+  </si>
+  <si>
+    <t>{rechnungsadresseOrganisation}</t>
   </si>
 </sst>
 </file>
@@ -328,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -361,6 +367,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -375,6 +384,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -690,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0BAE374-0165-43F7-9727-7ADA8430C8E9}">
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -701,32 +713,32 @@
     <col min="1" max="1" width="16.09765625" customWidth="1"/>
     <col min="2" max="2" width="16.19921875" customWidth="1"/>
     <col min="3" max="3" width="15.19921875" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="15.8984375" customWidth="1"/>
-    <col min="7" max="7" width="16.5" customWidth="1"/>
-    <col min="8" max="8" width="16.19921875" customWidth="1"/>
-    <col min="13" max="13" width="18.5" customWidth="1"/>
-    <col min="15" max="15" width="17.8984375" customWidth="1"/>
-    <col min="16" max="17" width="32" customWidth="1"/>
-    <col min="18" max="18" width="24" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="31.8984375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="34.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="15.8984375" customWidth="1"/>
+    <col min="8" max="8" width="16.5" customWidth="1"/>
+    <col min="9" max="9" width="16.19921875" customWidth="1"/>
+    <col min="14" max="14" width="18.5" customWidth="1"/>
+    <col min="16" max="16" width="17.8984375" customWidth="1"/>
+    <col min="17" max="18" width="32" customWidth="1"/>
+    <col min="19" max="19" width="24" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31.8984375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="34.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
@@ -735,62 +747,63 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="16" t="s">
+      <c r="C6" s="20"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
       <c r="K6" s="20"/>
-      <c r="L6" s="16" t="s">
+      <c r="L6" s="21"/>
+      <c r="M6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="16" t="s">
+      <c r="N6" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="16" t="s">
+      <c r="O6" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="O6" s="16" t="s">
+      <c r="P6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="P6" s="16" t="s">
+      <c r="Q6" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="Q6" s="16" t="s">
+      <c r="R6" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="R6" s="16" t="s">
+      <c r="S6" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="S6" s="13" t="s">
+      <c r="T6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="T6" s="13" t="s">
+      <c r="U6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="U6" s="13" t="s">
+      <c r="V6" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
@@ -800,37 +813,40 @@
       <c r="D7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="18"/>
+      <c r="F7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="L7" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="14"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
       <c r="T7" s="14"/>
       <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -852,65 +868,68 @@
       <c r="G8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="J8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="K8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="L8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="8" t="s">
+      <c r="M8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="M8" s="9" t="s">
+      <c r="N8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="O8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="O8" s="9" t="s">
+      <c r="P8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="P8" s="15" t="s">
+      <c r="Q8" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="Q8" s="15" t="s">
+      <c r="R8" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="R8" s="9" t="s">
+      <c r="S8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="S8" s="6" t="s">
+      <c r="T8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="T8" s="10" t="s">
+      <c r="U8" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="U8" s="10" t="s">
+      <c r="V8" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="S6:S7"/>
     <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="F6:L6"/>
+    <mergeCell ref="R6:R7"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="E6:E7"/>
-    <mergeCell ref="L6:L7"/>
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="N6:N7"/>
     <mergeCell ref="O6:O7"/>
-    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="P6:P7"/>
     <mergeCell ref="B6:D6"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="P6:P7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>